<commit_message>
update FDRs excel file
git-svn-id: file://localhost/tmp/svn2git/svn@5548 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/data-intensive-bio/results/FDRs.xlsx
+++ b/papers/data-intensive-bio/results/FDRs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1700" yWindow="600" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>